<commit_message>
add notebook part1 cleaning data
</commit_message>
<xml_diff>
--- a/raw_data/cities.xlsx
+++ b/raw_data/cities.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://knowyourpeople-my.sharepoint.com/personal/jrobert_knowyourpeople_fr/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jules\Documents\Github\function_tips\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{8B143129-42D5-483C-8C3D-BA40CDCCCB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79BCA5E0-327F-40C5-A5EF-C54D9D42BE28}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065ACEF1-1302-4034-B0FA-793C89064BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CDE1367F-F594-4840-9269-11C3F249D2AC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Donnée propre" sheetId="1" r:id="rId1"/>
-    <sheet name="Donnée à nettoyer" sheetId="2" r:id="rId2"/>
+    <sheet name="0. Data cleaned" sheetId="1" r:id="rId1"/>
+    <sheet name="1. Data to clean" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="40">
   <si>
     <t>City</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>euros</t>
+  </si>
+  <si>
+    <t>contact</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H11"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -830,15 +833,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7202329-7C7B-4D14-9963-B6A1770C7C72}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="14.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -863,8 +869,11 @@
       <c r="H1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -872,7 +881,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
         <v>105000</v>
@@ -890,7 +899,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -916,7 +925,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -936,13 +945,13 @@
         <v>66.2</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -968,7 +977,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -994,7 +1003,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1020,7 +1029,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1046,7 +1055,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1071,8 +1080,11 @@
       <c r="H9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>5960023</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1098,7 +1110,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1124,7 +1136,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1150,7 +1162,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1176,7 +1188,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1202,7 +1214,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1225,7 +1237,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1251,7 +1263,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1271,10 +1283,13 @@
         <v>562</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="H17" t="s">
         <v>33</v>
+      </c>
+      <c r="I17">
+        <v>35206512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>